<commit_message>
Before moving all packet communication to PacketCommunicator
</commit_message>
<xml_diff>
--- a/aapi/prirazeni_pdz+det.xlsx
+++ b/aapi/prirazeni_pdz+det.xlsx
@@ -8244,7 +8244,7 @@
   <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8304,10 +8304,10 @@
         <v>413</v>
       </c>
       <c r="G2" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="13">
         <v>513</v>
@@ -8329,7 +8329,7 @@
         <v>414</v>
       </c>
       <c r="G3" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="13">
         <v>1</v>
@@ -8354,7 +8354,7 @@
         <v>415</v>
       </c>
       <c r="G4" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H4" s="13">
         <v>0</v>
@@ -8379,10 +8379,10 @@
         <v>416</v>
       </c>
       <c r="G5" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H5" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="13">
         <v>513</v>
@@ -8404,10 +8404,10 @@
         <v>417</v>
       </c>
       <c r="G6" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="13">
         <v>513</v>
@@ -8429,7 +8429,7 @@
         <v>418</v>
       </c>
       <c r="G7" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="13">
         <v>1</v>
@@ -8454,7 +8454,7 @@
         <v>419</v>
       </c>
       <c r="G8" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H8" s="13">
         <v>0</v>
@@ -8479,10 +8479,10 @@
         <v>420</v>
       </c>
       <c r="G9" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H9" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="13">
         <v>513</v>
@@ -8504,10 +8504,10 @@
         <v>421</v>
       </c>
       <c r="G10" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="13">
         <v>513</v>
@@ -8529,7 +8529,7 @@
         <v>422</v>
       </c>
       <c r="G11" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11" s="13">
         <v>1</v>
@@ -8554,7 +8554,7 @@
         <v>423</v>
       </c>
       <c r="G12" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H12" s="13">
         <v>0</v>
@@ -8579,10 +8579,10 @@
         <v>424</v>
       </c>
       <c r="G13" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H13" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="13">
         <v>513</v>
@@ -8604,10 +8604,10 @@
         <v>425</v>
       </c>
       <c r="G14" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H14" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="13">
         <v>513</v>
@@ -8629,7 +8629,7 @@
         <v>426</v>
       </c>
       <c r="G15" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H15" s="13">
         <v>1</v>
@@ -8654,7 +8654,7 @@
         <v>427</v>
       </c>
       <c r="G16" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H16" s="13">
         <v>0</v>
@@ -8679,10 +8679,10 @@
         <v>428</v>
       </c>
       <c r="G17" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H17" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="13">
         <v>513</v>
@@ -8704,7 +8704,7 @@
         <v>429</v>
       </c>
       <c r="G18" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H18" s="13">
         <v>0</v>
@@ -8729,10 +8729,10 @@
         <v>430</v>
       </c>
       <c r="G19" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H19" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" s="13">
         <v>513</v>
@@ -8754,10 +8754,10 @@
         <v>431</v>
       </c>
       <c r="G20" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H20" s="13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I20" s="13">
         <v>513</v>
@@ -8779,7 +8779,7 @@
         <v>432</v>
       </c>
       <c r="G21" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H21" s="13">
         <v>0</v>
@@ -8804,10 +8804,10 @@
         <v>433</v>
       </c>
       <c r="G22" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H22" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" s="13">
         <v>512</v>
@@ -8829,10 +8829,10 @@
         <v>434</v>
       </c>
       <c r="G23" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H23" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="13">
         <v>512</v>
@@ -8854,7 +8854,7 @@
         <v>435</v>
       </c>
       <c r="G24" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H24" s="13">
         <v>1</v>
@@ -8879,7 +8879,7 @@
         <v>436</v>
       </c>
       <c r="G25" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H25" s="13">
         <v>0</v>
@@ -8904,10 +8904,10 @@
         <v>437</v>
       </c>
       <c r="G26" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H26" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" s="13">
         <v>512</v>
@@ -8929,10 +8929,10 @@
         <v>438</v>
       </c>
       <c r="G27" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H27" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="13">
         <v>512</v>
@@ -8954,7 +8954,7 @@
         <v>439</v>
       </c>
       <c r="G28" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H28" s="13">
         <v>1</v>
@@ -8979,7 +8979,7 @@
         <v>440</v>
       </c>
       <c r="G29" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H29" s="13">
         <v>0</v>
@@ -9004,10 +9004,10 @@
         <v>441</v>
       </c>
       <c r="G30" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H30" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" s="13">
         <v>512</v>
@@ -9029,10 +9029,10 @@
         <v>442</v>
       </c>
       <c r="G31" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H31" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="13">
         <v>512</v>
@@ -9054,7 +9054,7 @@
         <v>443</v>
       </c>
       <c r="G32" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H32" s="13">
         <v>1</v>
@@ -9079,7 +9079,7 @@
         <v>444</v>
       </c>
       <c r="G33" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H33" s="13">
         <v>0</v>
@@ -9104,10 +9104,10 @@
         <v>445</v>
       </c>
       <c r="G34" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H34" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" s="13">
         <v>512</v>
@@ -9129,7 +9129,7 @@
         <v>446</v>
       </c>
       <c r="G35" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H35" s="13">
         <v>0</v>
@@ -9154,10 +9154,10 @@
         <v>447</v>
       </c>
       <c r="G36" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H36" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" s="13">
         <v>512</v>
@@ -9179,10 +9179,10 @@
         <v>448</v>
       </c>
       <c r="G37" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H37" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="13">
         <v>512</v>
@@ -9204,7 +9204,7 @@
         <v>449</v>
       </c>
       <c r="G38" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H38" s="13">
         <v>1</v>
@@ -9229,10 +9229,10 @@
         <v>450</v>
       </c>
       <c r="G39" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H39" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" s="13">
         <v>512</v>
@@ -9254,7 +9254,7 @@
         <v>451</v>
       </c>
       <c r="G40" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H40" s="13">
         <v>1</v>
@@ -9279,7 +9279,7 @@
         <v>452</v>
       </c>
       <c r="G41" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H41" s="13">
         <v>0</v>
@@ -9304,10 +9304,10 @@
         <v>453</v>
       </c>
       <c r="G42" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H42" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" s="13">
         <v>514</v>
@@ -9329,10 +9329,10 @@
         <v>454</v>
       </c>
       <c r="G43" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H43" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43" s="13">
         <v>514</v>
@@ -9354,7 +9354,7 @@
         <v>455</v>
       </c>
       <c r="G44" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H44" s="13">
         <v>1</v>
@@ -9379,10 +9379,10 @@
         <v>456</v>
       </c>
       <c r="G45" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H45" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I45" s="13">
         <v>514</v>
@@ -9404,7 +9404,7 @@
         <v>457</v>
       </c>
       <c r="G46" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H46" s="13">
         <v>0</v>
@@ -9429,10 +9429,10 @@
         <v>458</v>
       </c>
       <c r="G47" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H47" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47" s="13">
         <v>514</v>
@@ -9454,10 +9454,10 @@
         <v>459</v>
       </c>
       <c r="G48" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H48" s="13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I48" s="13">
         <v>514</v>
@@ -9479,7 +9479,7 @@
         <v>460</v>
       </c>
       <c r="G49" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H49" s="13">
         <v>0</v>
@@ -9504,10 +9504,10 @@
         <v>461</v>
       </c>
       <c r="G50" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H50" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" s="13">
         <v>514</v>
@@ -9529,10 +9529,10 @@
         <v>462</v>
       </c>
       <c r="G51" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H51" s="13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I51" s="13">
         <v>514</v>
@@ -9554,7 +9554,7 @@
         <v>463</v>
       </c>
       <c r="G52" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H52" s="13">
         <v>0</v>
@@ -9579,10 +9579,10 @@
         <v>464</v>
       </c>
       <c r="G53" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H53" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" s="13">
         <v>514</v>
@@ -9604,10 +9604,10 @@
         <v>465</v>
       </c>
       <c r="G54" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H54" s="13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I54" s="13">
         <v>514</v>
@@ -9629,10 +9629,10 @@
         <v>466</v>
       </c>
       <c r="G55" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H55" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55" s="13">
         <v>514</v>
@@ -9654,7 +9654,7 @@
         <v>467</v>
       </c>
       <c r="G56" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H56" s="13">
         <v>1</v>
@@ -9679,10 +9679,10 @@
         <v>468</v>
       </c>
       <c r="G57" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H57" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I57" s="13">
         <v>514</v>
@@ -9704,10 +9704,10 @@
         <v>469</v>
       </c>
       <c r="G58" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H58" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58" s="13">
         <v>514</v>
@@ -9729,7 +9729,7 @@
         <v>470</v>
       </c>
       <c r="G59" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H59" s="13">
         <v>1</v>
@@ -9754,7 +9754,7 @@
         <v>471</v>
       </c>
       <c r="G60" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H60" s="13">
         <v>0</v>
@@ -9779,10 +9779,10 @@
         <v>472</v>
       </c>
       <c r="G61" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H61" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" s="13">
         <v>515</v>
@@ -9804,10 +9804,10 @@
         <v>473</v>
       </c>
       <c r="G62" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H62" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62" s="13">
         <v>515</v>
@@ -9829,7 +9829,7 @@
         <v>474</v>
       </c>
       <c r="G63" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H63" s="13">
         <v>1</v>
@@ -9854,7 +9854,7 @@
         <v>475</v>
       </c>
       <c r="G64" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H64" s="13">
         <v>0</v>
@@ -9879,10 +9879,10 @@
         <v>476</v>
       </c>
       <c r="G65" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H65" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" s="13">
         <v>515</v>
@@ -9904,10 +9904,10 @@
         <v>477</v>
       </c>
       <c r="G66" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H66" s="13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I66" s="13">
         <v>515</v>
@@ -9929,10 +9929,10 @@
         <v>478</v>
       </c>
       <c r="G67" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H67" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67" s="13">
         <v>515</v>
@@ -9954,7 +9954,7 @@
         <v>479</v>
       </c>
       <c r="G68" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H68" s="13">
         <v>1</v>
@@ -9979,7 +9979,7 @@
         <v>480</v>
       </c>
       <c r="G69" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H69" s="13">
         <v>0</v>
@@ -10004,10 +10004,10 @@
         <v>481</v>
       </c>
       <c r="G70" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H70" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I70" s="13">
         <v>515</v>
@@ -10029,10 +10029,10 @@
         <v>482</v>
       </c>
       <c r="G71" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H71" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I71" s="13">
         <v>515</v>
@@ -10054,7 +10054,7 @@
         <v>483</v>
       </c>
       <c r="G72" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H72" s="13">
         <v>1</v>
@@ -10079,7 +10079,7 @@
         <v>484</v>
       </c>
       <c r="G73" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H73" s="13">
         <v>0</v>
@@ -10104,10 +10104,10 @@
         <v>485</v>
       </c>
       <c r="G74" s="13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H74" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I74" s="13">
         <v>515</v>
@@ -10129,10 +10129,10 @@
         <v>486</v>
       </c>
       <c r="G75" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H75" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I75" s="13">
         <v>515</v>
@@ -10154,7 +10154,7 @@
         <v>487</v>
       </c>
       <c r="G76" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H76" s="13">
         <v>1</v>

</xml_diff>